<commit_message>
Se agregan las campos para los consecutivos y las observaciones de gabi
</commit_message>
<xml_diff>
--- a/Observaciones_NewViáticos_04-03-2019 - Editable.xlsx
+++ b/Observaciones_NewViáticos_04-03-2019 - Editable.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Datos PC\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\@Freelance\@IICA\Proyectos\Permisos_Vacaciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2556B02A-C934-477E-B3AA-55BCE2A026CC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25890" windowHeight="10230"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Observaciones" sheetId="1" r:id="rId1"/>
@@ -19,23 +20,17 @@
     <sheet name="5" sheetId="5" r:id="rId5"/>
     <sheet name="11" sheetId="8" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="78">
   <si>
     <t>Nombre del Proyecto:</t>
   </si>
@@ -274,7 +269,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
@@ -619,16 +614,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -653,7 +645,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="4" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="4" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -662,13 +654,13 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="8" fontId="4" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="4" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="1" applyBorder="1"/>
@@ -676,17 +668,17 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="6" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="6" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="8" fontId="4" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="4" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -705,61 +697,14 @@
     <xf numFmtId="8" fontId="6" fillId="10" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="8" fontId="4" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="8" fontId="6" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -769,42 +714,84 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -839,7 +826,7 @@
         <xdr:cNvPr id="2" name="Imagen 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{731690DC-C355-D94A-AC38-633C6C0A1B82}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{731690DC-C355-D94A-AC38-633C6C0A1B82}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -888,7 +875,7 @@
         <xdr:cNvPr id="2" name="Imagen 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9DEAF8A8-BED6-6445-B6D1-43F03C3B2614}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DEAF8A8-BED6-6445-B6D1-43F03C3B2614}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -932,7 +919,7 @@
         <xdr:cNvPr id="3" name="Llamada de flecha a la derecha 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5A6F8A51-40DC-4C42-A266-CDE2ADB89120}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A6F8A51-40DC-4C42-A266-CDE2ADB89120}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1003,7 +990,7 @@
         <xdr:cNvPr id="4" name="Recortar rectángulo de esquina sencilla 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E86B657A-9EF2-B347-BC0D-45F436238354}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E86B657A-9EF2-B347-BC0D-45F436238354}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1098,7 +1085,7 @@
         <xdr:cNvPr id="2" name="Imagen 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5182411D-C914-B644-9F1B-1426C35797A7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5182411D-C914-B644-9F1B-1426C35797A7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1142,7 +1129,7 @@
         <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F233B5B1-8D2B-E243-B27E-73A2419B406F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F233B5B1-8D2B-E243-B27E-73A2419B406F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1186,7 +1173,7 @@
         <xdr:cNvPr id="4" name="Imagen 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7AFCDF50-C30C-F54A-85D0-665AC9C9F947}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7AFCDF50-C30C-F54A-85D0-665AC9C9F947}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1230,7 +1217,7 @@
         <xdr:cNvPr id="5" name="Imagen 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2DB2FC9A-6BC8-DB4C-BCF9-F95488E0DA2B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DB2FC9A-6BC8-DB4C-BCF9-F95488E0DA2B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1279,7 +1266,7 @@
         <xdr:cNvPr id="2" name="Imagen 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3E9AD14D-2122-E343-AC85-990D520A0989}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E9AD14D-2122-E343-AC85-990D520A0989}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1332,7 +1319,7 @@
         <xdr:cNvPr id="2" name="Imagen 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B6B5FB32-8B26-D442-9483-4C03B740F937}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6B5FB32-8B26-D442-9483-4C03B740F937}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1376,7 +1363,7 @@
         <xdr:cNvPr id="4" name="Recortar rectángulo de esquina sencilla 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{15F6F4CC-0B9B-B948-B905-87061A1F3169}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15F6F4CC-0B9B-B948-B905-87061A1F3169}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1469,7 +1456,7 @@
         <xdr:cNvPr id="5" name="Imagen 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B6330ECB-C2DE-F14F-9555-73179FEBB0D3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6330ECB-C2DE-F14F-9555-73179FEBB0D3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1513,7 +1500,7 @@
         <xdr:cNvPr id="9" name="Elipse 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A9775A8E-DDBE-334E-8873-E76C415850CC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9775A8E-DDBE-334E-8873-E76C415850CC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1577,7 +1564,7 @@
         <xdr:cNvPr id="10" name="Elipse 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{96EDFB90-714E-D049-8B41-22B184A607A0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96EDFB90-714E-D049-8B41-22B184A607A0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1641,7 +1628,7 @@
         <xdr:cNvPr id="11" name="Imagen 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{843852D7-5B71-0048-B22E-342C960938D5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{843852D7-5B71-0048-B22E-342C960938D5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1685,7 +1672,7 @@
         <xdr:cNvPr id="12" name="Elipse 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F26B8AEF-F3A6-8A44-9DFB-E9103BB5EFA4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F26B8AEF-F3A6-8A44-9DFB-E9103BB5EFA4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1749,7 +1736,7 @@
         <xdr:cNvPr id="13" name="Elipse 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{53C9C820-2000-B349-BCA6-80E4589BE4A6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53C9C820-2000-B349-BCA6-80E4589BE4A6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1813,7 +1800,7 @@
         <xdr:cNvPr id="14" name="Llamada de flecha a la derecha 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6424201D-683A-E847-82A3-144BC31B8BCD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6424201D-683A-E847-82A3-144BC31B8BCD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1889,7 +1876,7 @@
         <xdr:cNvPr id="2" name="Imagen 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{057E7506-69DA-B049-9786-1197B10CDC2C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{057E7506-69DA-B049-9786-1197B10CDC2C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1933,7 +1920,7 @@
         <xdr:cNvPr id="3" name="Llamada de flecha a la derecha 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{87AB7312-A355-E54D-9C5B-6AE512E3344D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87AB7312-A355-E54D-9C5B-6AE512E3344D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2004,7 +1991,7 @@
         <xdr:cNvPr id="4" name="Recortar rectángulo de esquina sencilla 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{177BFE0D-EF5A-744F-AEC5-09BD8EFE719E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{177BFE0D-EF5A-744F-AEC5-09BD8EFE719E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2386,72 +2373,67 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" topLeftCell="B5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.375" customWidth="1"/>
-    <col min="2" max="2" width="5.875" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.375" style="40" customWidth="1"/>
+    <col min="2" max="2" width="5.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.375" style="38" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
     <col min="5" max="5" width="29.875" customWidth="1"/>
     <col min="6" max="6" width="28" customWidth="1"/>
-    <col min="7" max="7" width="37.125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.125" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.625" customWidth="1"/>
     <col min="9" max="9" width="27.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="43"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="43"/>
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="51"/>
+      <c r="D3" s="53"/>
       <c r="E3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="43"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="43"/>
-      <c r="C4" s="51" t="s">
+      <c r="C4" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="51"/>
-      <c r="G4" s="43"/>
+      <c r="D4" s="53"/>
     </row>
     <row r="10" spans="2:9" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="56" t="s">
+      <c r="C10" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="56"/>
-      <c r="E10" s="56"/>
-      <c r="F10" s="42" t="s">
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="G10" s="42" t="s">
+      <c r="G10" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="H10" s="42" t="s">
+      <c r="H10" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="I10" s="42" t="s">
+      <c r="I10" s="39" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2459,19 +2441,19 @@
       <c r="B11" s="3">
         <v>1</v>
       </c>
-      <c r="C11" s="45" t="s">
+      <c r="C11" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="45"/>
-      <c r="E11" s="45"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="54"/>
       <c r="F11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="44" t="s">
+      <c r="G11" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="H11" s="59" t="s">
-        <v>73</v>
+      <c r="H11" s="45" t="s">
+        <v>76</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>11</v>
@@ -2481,19 +2463,19 @@
       <c r="B12" s="3">
         <v>2</v>
       </c>
-      <c r="C12" s="45" t="s">
+      <c r="C12" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="45"/>
-      <c r="E12" s="45"/>
+      <c r="D12" s="54"/>
+      <c r="E12" s="54"/>
       <c r="F12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="H12" s="61" t="s">
-        <v>74</v>
+      <c r="H12" s="45" t="s">
+        <v>76</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>11</v>
@@ -2503,19 +2485,19 @@
       <c r="B13" s="3">
         <v>3</v>
       </c>
-      <c r="C13" s="45" t="s">
+      <c r="C13" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="54"/>
       <c r="F13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="44" t="s">
+      <c r="G13" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="H13" s="59" t="s">
-        <v>73</v>
+      <c r="H13" s="45" t="s">
+        <v>76</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>11</v>
@@ -2525,16 +2507,16 @@
       <c r="B14" s="3">
         <v>4</v>
       </c>
-      <c r="C14" s="45" t="s">
+      <c r="C14" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
+      <c r="D14" s="54"/>
+      <c r="E14" s="54"/>
       <c r="F14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="62"/>
-      <c r="H14" s="63" t="s">
+      <c r="G14" s="44"/>
+      <c r="H14" s="45" t="s">
         <v>76</v>
       </c>
       <c r="I14" s="2" t="s">
@@ -2545,18 +2527,20 @@
       <c r="B15" s="3">
         <v>5</v>
       </c>
-      <c r="C15" s="45" t="s">
+      <c r="C15" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="45"/>
-      <c r="E15" s="45"/>
+      <c r="D15" s="54"/>
+      <c r="E15" s="54"/>
       <c r="F15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G15" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H15" s="61"/>
+      <c r="H15" s="45" t="s">
+        <v>76</v>
+      </c>
       <c r="I15" s="2" t="s">
         <v>11</v>
       </c>
@@ -2565,40 +2549,40 @@
       <c r="B16" s="3">
         <v>6</v>
       </c>
-      <c r="C16" s="45" t="s">
+      <c r="C16" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="45"/>
-      <c r="E16" s="45"/>
+      <c r="D16" s="54"/>
+      <c r="E16" s="54"/>
       <c r="F16" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G16" s="44" t="s">
+      <c r="G16" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="H16" s="59" t="s">
-        <v>73</v>
+      <c r="H16" s="45" t="s">
+        <v>76</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="17" spans="2:9" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B17" s="4">
+      <c r="B17" s="3">
         <v>7</v>
       </c>
-      <c r="C17" s="45" t="s">
+      <c r="C17" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="54"/>
       <c r="F17" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G17" s="44" t="s">
+      <c r="G17" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="H17" s="59" t="s">
+      <c r="H17" s="41" t="s">
         <v>73</v>
       </c>
       <c r="I17" s="2" t="s">
@@ -2606,21 +2590,21 @@
       </c>
     </row>
     <row r="18" spans="2:9" ht="89.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="4">
+      <c r="B18" s="3">
         <v>8</v>
       </c>
-      <c r="C18" s="45" t="s">
+      <c r="C18" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="45"/>
-      <c r="E18" s="45"/>
+      <c r="D18" s="54"/>
+      <c r="E18" s="54"/>
       <c r="F18" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G18" s="62" t="s">
+      <c r="G18" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="H18" s="63" t="s">
+      <c r="H18" s="45" t="s">
         <v>76</v>
       </c>
       <c r="I18" s="2" t="s">
@@ -2628,95 +2612,95 @@
       </c>
     </row>
     <row r="19" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="4">
+      <c r="B19" s="3">
         <v>9</v>
       </c>
-      <c r="C19" s="52" t="s">
+      <c r="C19" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="52"/>
-      <c r="E19" s="52"/>
+      <c r="D19" s="67"/>
+      <c r="E19" s="67"/>
       <c r="F19" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G19" s="62" t="s">
+      <c r="G19" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="H19" s="63"/>
+      <c r="H19" s="45"/>
       <c r="I19" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="20" spans="2:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="4">
+      <c r="B20" s="3">
         <v>10</v>
       </c>
-      <c r="C20" s="46" t="s">
+      <c r="C20" s="68" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="46"/>
-      <c r="E20" s="46"/>
+      <c r="D20" s="68"/>
+      <c r="E20" s="68"/>
       <c r="F20" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G20" s="62"/>
-      <c r="H20" s="63"/>
+      <c r="G20" s="44"/>
+      <c r="H20" s="45"/>
       <c r="I20" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="21" spans="2:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="4">
+      <c r="B21" s="3">
         <v>11</v>
       </c>
-      <c r="C21" s="47" t="s">
+      <c r="C21" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="48"/>
-      <c r="E21" s="49"/>
+      <c r="D21" s="65"/>
+      <c r="E21" s="66"/>
       <c r="F21" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G21" s="62" t="s">
+      <c r="G21" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="H21" s="63"/>
+      <c r="H21" s="45"/>
       <c r="I21" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="22" spans="2:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="4">
+      <c r="B22" s="3">
         <v>12</v>
       </c>
-      <c r="C22" s="53" t="s">
+      <c r="C22" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="D22" s="54"/>
-      <c r="E22" s="55"/>
+      <c r="D22" s="49"/>
+      <c r="E22" s="50"/>
       <c r="F22" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G22" s="62"/>
-      <c r="H22" s="63"/>
+      <c r="G22" s="44"/>
+      <c r="H22" s="45"/>
       <c r="I22" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="23" spans="2:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="4">
+      <c r="B23" s="3">
         <v>13</v>
       </c>
-      <c r="C23" s="53" t="s">
+      <c r="C23" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="D23" s="54"/>
-      <c r="E23" s="55"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="50"/>
       <c r="F23" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G23" s="6"/>
-      <c r="H23" s="61" t="s">
+      <c r="G23" s="5"/>
+      <c r="H23" s="43" t="s">
         <v>74</v>
       </c>
       <c r="I23" s="2" t="s">
@@ -2724,37 +2708,37 @@
       </c>
     </row>
     <row r="24" spans="2:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="4">
+      <c r="B24" s="3">
         <v>14</v>
       </c>
-      <c r="C24" s="47" t="s">
+      <c r="C24" s="64" t="s">
         <v>31</v>
       </c>
-      <c r="D24" s="48"/>
-      <c r="E24" s="49"/>
+      <c r="D24" s="65"/>
+      <c r="E24" s="66"/>
       <c r="F24" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G24" s="6" t="s">
+      <c r="G24" s="5" t="s">
         <v>32</v>
       </c>
       <c r="H24" s="2"/>
-      <c r="I24" s="41" t="s">
+      <c r="I24" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="25" spans="2:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="6">
+      <c r="B25" s="5">
         <v>15</v>
       </c>
-      <c r="C25" s="45" t="s">
+      <c r="C25" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="D25" s="45"/>
-      <c r="E25" s="45"/>
-      <c r="F25" s="39"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="61" t="s">
+      <c r="D25" s="54"/>
+      <c r="E25" s="54"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="43" t="s">
         <v>74</v>
       </c>
       <c r="I25" s="2" t="s">
@@ -2762,86 +2746,86 @@
       </c>
     </row>
     <row r="26" spans="2:9" ht="47.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="6">
+      <c r="B26" s="5">
         <v>16</v>
       </c>
-      <c r="C26" s="64" t="s">
+      <c r="C26" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="D26" s="64"/>
-      <c r="E26" s="64"/>
-      <c r="F26" s="60" t="s">
+      <c r="D26" s="63"/>
+      <c r="E26" s="63"/>
+      <c r="F26" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="G26" s="65"/>
-      <c r="H26" s="60"/>
-      <c r="I26" s="60" t="s">
+      <c r="G26" s="46"/>
+      <c r="H26" s="42"/>
+      <c r="I26" s="42" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="27" spans="2:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="6">
+      <c r="B27" s="5">
         <v>17</v>
       </c>
-      <c r="C27" s="66" t="s">
+      <c r="C27" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="D27" s="66"/>
-      <c r="E27" s="66"/>
-      <c r="F27" s="67" t="s">
+      <c r="D27" s="62"/>
+      <c r="E27" s="62"/>
+      <c r="F27" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="G27" s="65"/>
-      <c r="H27" s="60"/>
-      <c r="I27" s="60" t="s">
+      <c r="G27" s="46"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="42" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="28" spans="2:9" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="6">
+      <c r="B28" s="5">
         <v>18</v>
       </c>
-      <c r="C28" s="68" t="s">
+      <c r="C28" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="D28" s="69"/>
-      <c r="E28" s="70"/>
-      <c r="F28" s="60"/>
-      <c r="G28" s="65"/>
-      <c r="H28" s="60"/>
-      <c r="I28" s="60" t="s">
+      <c r="D28" s="56"/>
+      <c r="E28" s="57"/>
+      <c r="F28" s="42"/>
+      <c r="G28" s="46"/>
+      <c r="H28" s="42"/>
+      <c r="I28" s="42" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="29" spans="2:9" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="6">
+      <c r="B29" s="5">
         <v>19</v>
       </c>
-      <c r="C29" s="68" t="s">
+      <c r="C29" s="55" t="s">
         <v>40</v>
       </c>
-      <c r="D29" s="69"/>
-      <c r="E29" s="70"/>
-      <c r="F29" s="60"/>
-      <c r="G29" s="65"/>
-      <c r="H29" s="60"/>
-      <c r="I29" s="60"/>
+      <c r="D29" s="56"/>
+      <c r="E29" s="57"/>
+      <c r="F29" s="42"/>
+      <c r="G29" s="46"/>
+      <c r="H29" s="42"/>
+      <c r="I29" s="42"/>
     </row>
     <row r="30" spans="2:9" ht="62.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="6">
+      <c r="B30" s="5">
         <v>20</v>
       </c>
-      <c r="C30" s="71" t="s">
+      <c r="C30" s="58" t="s">
         <v>41</v>
       </c>
-      <c r="D30" s="71"/>
-      <c r="E30" s="71"/>
-      <c r="F30" s="67" t="s">
+      <c r="D30" s="58"/>
+      <c r="E30" s="58"/>
+      <c r="F30" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="G30" s="65"/>
-      <c r="H30" s="60"/>
-      <c r="I30" s="60" t="s">
+      <c r="G30" s="46"/>
+      <c r="H30" s="42"/>
+      <c r="I30" s="42" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2849,31 +2833,22 @@
       <c r="B31" s="3">
         <v>21</v>
       </c>
-      <c r="C31" s="72" t="s">
+      <c r="C31" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="D31" s="73"/>
-      <c r="E31" s="74"/>
-      <c r="F31" s="60" t="s">
+      <c r="D31" s="60"/>
+      <c r="E31" s="61"/>
+      <c r="F31" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="G31" s="65"/>
-      <c r="H31" s="60"/>
-      <c r="I31" s="60" t="s">
+      <c r="G31" s="46"/>
+      <c r="H31" s="42"/>
+      <c r="I31" s="42" t="s">
         <v>46</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="D1:H1"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
     <mergeCell ref="C28:E28"/>
     <mergeCell ref="C30:E30"/>
     <mergeCell ref="C31:E31"/>
@@ -2890,6 +2865,15 @@
     <mergeCell ref="C25:E25"/>
     <mergeCell ref="C21:E21"/>
     <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2897,7 +2881,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -2912,7 +2896,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="A44" workbookViewId="0">
@@ -2927,7 +2911,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2942,7 +2926,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A2:K27"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
@@ -2951,602 +2935,602 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="34.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5" style="7"/>
-    <col min="2" max="2" width="17" style="7" customWidth="1"/>
-    <col min="3" max="3" width="15" style="7" customWidth="1"/>
-    <col min="4" max="4" width="25.625" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.875" style="7" customWidth="1"/>
-    <col min="6" max="6" width="14.5" style="7" customWidth="1"/>
-    <col min="7" max="7" width="15.125" style="7" customWidth="1"/>
-    <col min="8" max="16384" width="11.5" style="7"/>
+    <col min="1" max="1" width="11.5" style="6"/>
+    <col min="2" max="2" width="17" style="6" customWidth="1"/>
+    <col min="3" max="3" width="15" style="6" customWidth="1"/>
+    <col min="4" max="4" width="25.625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.875" style="6" customWidth="1"/>
+    <col min="6" max="6" width="14.5" style="6" customWidth="1"/>
+    <col min="7" max="7" width="15.125" style="6" customWidth="1"/>
+    <col min="8" max="16384" width="11.5" style="6"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="57" t="s">
+      <c r="B2" s="69" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="57"/>
-      <c r="F2" s="57" t="s">
+      <c r="C2" s="69"/>
+      <c r="F2" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="G2" s="57"/>
+      <c r="G2" s="69"/>
     </row>
     <row r="3" spans="1:11" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="7" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="9">
         <v>980</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="9">
         <v>490</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="10">
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="9">
         <v>550</v>
       </c>
-      <c r="G4" s="10">
+      <c r="G4" s="9">
         <v>435</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="11">
         <v>1700</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="9">
         <v>850</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="9">
         <v>750</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="9">
         <v>625</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="K5" s="6" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="9">
         <v>2850</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="9">
         <v>1425</v>
       </c>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="15">
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="14">
         <v>925</v>
       </c>
-      <c r="G6" s="15">
+      <c r="G6" s="14">
         <v>900</v>
       </c>
-      <c r="K6" s="31">
+      <c r="K6" s="30">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="58"/>
-      <c r="B8" s="58"/>
-      <c r="C8" s="58"/>
-      <c r="D8" s="58"/>
+      <c r="A8" s="70"/>
+      <c r="B8" s="70"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="70"/>
     </row>
     <row r="9" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="F9" s="18"/>
-      <c r="G9" s="29" t="s">
+      <c r="F9" s="17"/>
+      <c r="G9" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="H9" s="32" t="s">
+      <c r="H9" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="I9" s="33" t="s">
+      <c r="I9" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="J9" s="7" t="s">
+      <c r="J9" s="6" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="B10" s="20">
+      <c r="B10" s="19">
         <v>980</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D10" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="6">
         <v>1</v>
       </c>
-      <c r="G10" s="30">
+      <c r="G10" s="29">
         <f>B10*K6</f>
         <v>4900</v>
       </c>
-      <c r="H10" s="22">
+      <c r="H10" s="21">
         <f>B10*0.5</f>
         <v>490</v>
       </c>
-      <c r="I10" s="34">
+      <c r="I10" s="33">
         <f>G10+H10</f>
         <v>5390</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="B11" s="24">
+      <c r="B11" s="23">
         <v>1700</v>
       </c>
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="D11" s="25" t="s">
+      <c r="D11" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="6">
         <v>1</v>
       </c>
-      <c r="G11" s="37">
+      <c r="G11" s="36">
         <f>B11*K6</f>
         <v>8500</v>
       </c>
-      <c r="H11" s="37">
+      <c r="H11" s="36">
         <f t="shared" ref="H11:H21" si="0">B11*0.5</f>
         <v>850</v>
       </c>
-      <c r="I11" s="38">
+      <c r="I11" s="37">
         <f t="shared" ref="I11:I21" si="1">G11+H11</f>
         <v>9350</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="B12" s="26">
+      <c r="B12" s="25">
         <v>2850</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C12" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="D12" s="25" t="s">
+      <c r="D12" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="6">
         <v>1</v>
       </c>
-      <c r="G12" s="30">
+      <c r="G12" s="29">
         <f>B12*K6</f>
         <v>14250</v>
       </c>
-      <c r="H12" s="22">
+      <c r="H12" s="21">
         <f t="shared" si="0"/>
         <v>1425</v>
       </c>
-      <c r="I12" s="34">
+      <c r="I12" s="33">
         <f t="shared" si="1"/>
         <v>15675</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="23" t="s">
+      <c r="A13" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="B13" s="26">
+      <c r="B13" s="25">
         <v>490</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="D13" s="25" t="s">
+      <c r="D13" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="6">
         <v>1</v>
       </c>
-      <c r="G13" s="30">
+      <c r="G13" s="29">
         <f>B13*K6</f>
         <v>2450</v>
       </c>
-      <c r="H13" s="22">
+      <c r="H13" s="21">
         <f t="shared" si="0"/>
         <v>245</v>
       </c>
-      <c r="I13" s="34">
+      <c r="I13" s="33">
         <f t="shared" si="1"/>
         <v>2695</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="B14" s="26">
+      <c r="B14" s="25">
         <v>850</v>
       </c>
-      <c r="C14" s="25" t="s">
+      <c r="C14" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="D14" s="25" t="s">
+      <c r="D14" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="6">
         <v>1</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F14" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="G14" s="30">
+      <c r="G14" s="29">
         <f>B14*K6</f>
         <v>4250</v>
       </c>
-      <c r="H14" s="22">
+      <c r="H14" s="21">
         <f t="shared" si="0"/>
         <v>425</v>
       </c>
-      <c r="I14" s="34">
+      <c r="I14" s="33">
         <f t="shared" si="1"/>
         <v>4675</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="B15" s="26">
+      <c r="B15" s="25">
         <v>1425</v>
       </c>
-      <c r="C15" s="25" t="s">
+      <c r="C15" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="D15" s="25" t="s">
+      <c r="D15" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="6">
         <v>1</v>
       </c>
-      <c r="G15" s="30">
+      <c r="G15" s="29">
         <f>B15*K6</f>
         <v>7125</v>
       </c>
-      <c r="H15" s="22">
+      <c r="H15" s="21">
         <f t="shared" si="0"/>
         <v>712.5</v>
       </c>
-      <c r="I15" s="34">
+      <c r="I15" s="33">
         <f t="shared" si="1"/>
         <v>7837.5</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="B16" s="26">
+      <c r="B16" s="25">
         <v>550</v>
       </c>
-      <c r="C16" s="25" t="s">
+      <c r="C16" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="D16" s="25" t="s">
+      <c r="D16" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="6">
         <v>1</v>
       </c>
-      <c r="G16" s="35">
+      <c r="G16" s="34">
         <f>B16*K6</f>
         <v>2750</v>
       </c>
-      <c r="H16" s="35">
+      <c r="H16" s="34">
         <f t="shared" si="0"/>
         <v>275</v>
       </c>
-      <c r="I16" s="36">
+      <c r="I16" s="35">
         <f t="shared" si="1"/>
         <v>3025</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="23" t="s">
+      <c r="A17" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="B17" s="26">
+      <c r="B17" s="25">
         <v>750</v>
       </c>
-      <c r="C17" s="25" t="s">
+      <c r="C17" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="D17" s="25" t="s">
+      <c r="D17" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="6">
         <v>1</v>
       </c>
-      <c r="G17" s="30">
+      <c r="G17" s="29">
         <f>B17*K6</f>
         <v>3750</v>
       </c>
-      <c r="H17" s="22">
+      <c r="H17" s="21">
         <f t="shared" si="0"/>
         <v>375</v>
       </c>
-      <c r="I17" s="34">
+      <c r="I17" s="33">
         <f t="shared" si="1"/>
         <v>4125</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="23" t="s">
+      <c r="A18" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="B18" s="26">
+      <c r="B18" s="25">
         <v>925</v>
       </c>
-      <c r="C18" s="25" t="s">
+      <c r="C18" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="D18" s="25" t="s">
+      <c r="D18" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="6">
         <v>1</v>
       </c>
-      <c r="G18" s="30">
+      <c r="G18" s="29">
         <f>B18*K6</f>
         <v>4625</v>
       </c>
-      <c r="H18" s="22">
+      <c r="H18" s="21">
         <f t="shared" si="0"/>
         <v>462.5</v>
       </c>
-      <c r="I18" s="34">
+      <c r="I18" s="33">
         <f t="shared" si="1"/>
         <v>5087.5</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="26">
+      <c r="B19" s="25">
         <v>435</v>
       </c>
-      <c r="C19" s="25" t="s">
+      <c r="C19" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="D19" s="25" t="s">
+      <c r="D19" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="6">
         <v>1</v>
       </c>
-      <c r="G19" s="30">
+      <c r="G19" s="29">
         <f>B19*K6</f>
         <v>2175</v>
       </c>
-      <c r="H19" s="22">
+      <c r="H19" s="21">
         <f t="shared" si="0"/>
         <v>217.5</v>
       </c>
-      <c r="I19" s="34">
+      <c r="I19" s="33">
         <f t="shared" si="1"/>
         <v>2392.5</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="23" t="s">
+      <c r="A20" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="B20" s="26">
+      <c r="B20" s="25">
         <v>625</v>
       </c>
-      <c r="C20" s="25" t="s">
+      <c r="C20" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="D20" s="25" t="s">
+      <c r="D20" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="6">
         <v>1</v>
       </c>
-      <c r="G20" s="30">
+      <c r="G20" s="29">
         <f>B20*K6</f>
         <v>3125</v>
       </c>
-      <c r="H20" s="22">
+      <c r="H20" s="21">
         <f t="shared" si="0"/>
         <v>312.5</v>
       </c>
-      <c r="I20" s="34">
+      <c r="I20" s="33">
         <f t="shared" si="1"/>
         <v>3437.5</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="B21" s="26">
+      <c r="B21" s="25">
         <v>900</v>
       </c>
-      <c r="C21" s="25" t="s">
+      <c r="C21" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="D21" s="25" t="s">
+      <c r="D21" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="6">
         <v>1</v>
       </c>
-      <c r="G21" s="30">
+      <c r="G21" s="29">
         <f>B21*K6</f>
         <v>4500</v>
       </c>
-      <c r="H21" s="22">
+      <c r="H21" s="21">
         <f t="shared" si="0"/>
         <v>450</v>
       </c>
-      <c r="I21" s="34">
+      <c r="I21" s="33">
         <f t="shared" si="1"/>
         <v>4950</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="23" t="s">
+      <c r="A22" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="B22" s="27">
+      <c r="B22" s="26">
         <v>450</v>
       </c>
-      <c r="C22" s="28" t="s">
+      <c r="C22" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="D22" s="28" t="s">
+      <c r="D22" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="E22" s="7">
+      <c r="E22" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="23" t="s">
+      <c r="A23" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="B23" s="27">
+      <c r="B23" s="26">
         <v>225</v>
       </c>
-      <c r="C23" s="28" t="s">
+      <c r="C23" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="D23" s="28" t="s">
+      <c r="D23" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="23" t="s">
+      <c r="A24" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="B24" s="27">
+      <c r="B24" s="26">
         <v>450</v>
       </c>
-      <c r="C24" s="28" t="s">
+      <c r="C24" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="D24" s="28" t="s">
+      <c r="D24" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="23" t="s">
+      <c r="A25" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="B25" s="27">
+      <c r="B25" s="26">
         <v>225</v>
       </c>
-      <c r="C25" s="28" t="s">
+      <c r="C25" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="D25" s="28" t="s">
+      <c r="D25" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="E25" s="7">
+      <c r="E25" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="23" t="s">
+      <c r="A26" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="B26" s="27">
+      <c r="B26" s="26">
         <v>450</v>
       </c>
-      <c r="C26" s="28" t="s">
+      <c r="C26" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="D26" s="28" t="s">
+      <c r="D26" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="E26" s="7">
+      <c r="E26" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="23" t="s">
+      <c r="A27" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="B27" s="27">
+      <c r="B27" s="26">
         <v>225</v>
       </c>
-      <c r="C27" s="28" t="s">
+      <c r="C27" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="D27" s="28" t="s">
+      <c r="D27" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="E27" s="7">
+      <c r="E27" s="6">
         <v>2</v>
       </c>
     </row>
@@ -3563,7 +3547,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>